<commit_message>
add down post form
add down post form
</commit_message>
<xml_diff>
--- a/raw_data/chatbot_data_core.xlsx
+++ b/raw_data/chatbot_data_core.xlsx
@@ -804,7 +804,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E128"/>
+  <dimension ref="A1:D33"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -833,2052 +833,366 @@
           <t>Rasa-Stories</t>
         </is>
       </c>
-      <c r="E1" t="inlineStr"/>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>2</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>tôi muốn hạ tin hoàn tiền</t>
+          <t>Tôi muốn hạ tin hoàn tiền</t>
         </is>
       </c>
       <c r="C2" t="inlineStr"/>
       <c r="D2" t="inlineStr">
         <is>
-          <t>request_down_post</t>
-        </is>
-      </c>
-      <c r="E2" t="inlineStr"/>
+          <t>* request_down_post</t>
+        </is>
+      </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr"/>
       <c r="B3" t="inlineStr"/>
-      <c r="C3" t="inlineStr">
-        <is>
-          <t>Bạn liên hệ bộ phận chăm sóc khách hàng để được hỗ trợ hạ tin và hoàn tiền về tài khoản nhé.
-Bot chỉ giúp bạn tính toán số tiền được hoàn trả khi hạ tin thôi ạ! Bạn vui lòng cung cấp một số thông tin.</t>
-        </is>
-      </c>
+      <c r="C3" t="inlineStr"/>
       <c r="D3" t="inlineStr">
         <is>
-          <t>utter_bot_need_info_for_refund</t>
-        </is>
-      </c>
-      <c r="E3" t="inlineStr"/>
+          <t>- utter_bot_need_info_for_refund</t>
+        </is>
+      </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr"/>
       <c r="B4" t="inlineStr"/>
-      <c r="C4" t="inlineStr">
-        <is>
-          <t>Bạn đang dùng gói vip nào</t>
-        </is>
-      </c>
+      <c r="C4" t="inlineStr"/>
       <c r="D4" t="inlineStr">
         <is>
-          <t>utter_ask_source_post_package</t>
-        </is>
-      </c>
-      <c r="E4" t="inlineStr"/>
+          <t>- calculate_down_post_form</t>
+        </is>
+      </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr"/>
-      <c r="B5" t="inlineStr">
-        <is>
-          <t>gói vip 3</t>
-        </is>
-      </c>
+      <c r="B5" t="inlineStr"/>
       <c r="C5" t="inlineStr"/>
       <c r="D5" t="inlineStr">
         <is>
-          <t>enter_data</t>
-        </is>
-      </c>
-      <c r="E5" t="inlineStr"/>
+          <t>- form{"name": "calculate_down_post_form"}</t>
+        </is>
+      </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr"/>
       <c r="B6" t="inlineStr"/>
-      <c r="C6" t="inlineStr">
-        <is>
-          <t>action_set_source_post_package</t>
-        </is>
-      </c>
+      <c r="C6" t="inlineStr"/>
       <c r="D6" t="inlineStr">
         <is>
-          <t>action_set_source_post_package</t>
-        </is>
-      </c>
-      <c r="E6" t="inlineStr"/>
+          <t xml:space="preserve">- form{"name": null} </t>
+        </is>
+      </c>
     </row>
     <row r="7">
-      <c r="A7" t="inlineStr"/>
-      <c r="B7" t="inlineStr"/>
-      <c r="C7" t="inlineStr">
-        <is>
-          <t>Số ngày mua ban đầu là bao nhiêu?</t>
-        </is>
-      </c>
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>3</t>
+        </is>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>Tối muốn hạ tin hoàn tiền</t>
+        </is>
+      </c>
+      <c r="C7" t="inlineStr"/>
       <c r="D7" t="inlineStr">
         <is>
-          <t>utter_ask_buy_vip_duration</t>
-        </is>
-      </c>
-      <c r="E7" t="inlineStr"/>
+          <t>* request_down_post</t>
+        </is>
+      </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr"/>
-      <c r="B8" t="inlineStr">
-        <is>
-          <t>Mình mua 15 ngày</t>
-        </is>
-      </c>
+      <c r="B8" t="inlineStr"/>
       <c r="C8" t="inlineStr"/>
       <c r="D8" t="inlineStr">
         <is>
-          <t>enter_data</t>
-        </is>
-      </c>
-      <c r="E8" t="inlineStr"/>
+          <t>- utter_bot_need_info_for_refund</t>
+        </is>
+      </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr"/>
       <c r="B9" t="inlineStr"/>
-      <c r="C9" t="inlineStr">
-        <is>
-          <t>action_set_buy_vip_duration</t>
-        </is>
-      </c>
+      <c r="C9" t="inlineStr"/>
       <c r="D9" t="inlineStr">
         <is>
-          <t>action_set_buy_vip_duration</t>
-        </is>
-      </c>
-      <c r="E9" t="inlineStr"/>
+          <t>- calculate_down_post_form</t>
+        </is>
+      </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr"/>
       <c r="B10" t="inlineStr"/>
-      <c r="C10" t="inlineStr">
-        <is>
-          <t>Bạn đã sử dụng trong bao ngày rồi?</t>
-        </is>
-      </c>
+      <c r="C10" t="inlineStr"/>
       <c r="D10" t="inlineStr">
         <is>
-          <t>utter_ask_used_vip_duration</t>
-        </is>
-      </c>
-      <c r="E10" t="inlineStr"/>
+          <t>- form{"name":"calculate_down_post_form"}</t>
+        </is>
+      </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr"/>
-      <c r="B11" t="inlineStr">
-        <is>
-          <t>mời dùng có 3 ngày thôi</t>
-        </is>
-      </c>
+      <c r="B11" t="inlineStr"/>
       <c r="C11" t="inlineStr"/>
       <c r="D11" t="inlineStr">
         <is>
-          <t>enter_data</t>
-        </is>
-      </c>
-      <c r="E11" t="inlineStr"/>
+          <t>- slot{"requested_slot":"source_post_package"}</t>
+        </is>
+      </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr"/>
-      <c r="B12" t="inlineStr"/>
-      <c r="C12" t="inlineStr">
-        <is>
-          <t>action_set_used_vip_duration</t>
-        </is>
-      </c>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>Thế thôi ko cần đâu</t>
+        </is>
+      </c>
+      <c r="C12" t="inlineStr"/>
       <c r="D12" t="inlineStr">
         <is>
-          <t>action_set_used_vip_duration</t>
-        </is>
-      </c>
-      <c r="E12" t="inlineStr"/>
+          <t>* canthelp OR deny</t>
+        </is>
+      </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr"/>
       <c r="B13" t="inlineStr"/>
-      <c r="C13" t="inlineStr">
-        <is>
-          <t>Số tiền bạn được hoàn trả là ...</t>
-        </is>
-      </c>
+      <c r="C13" t="inlineStr"/>
       <c r="D13" t="inlineStr">
         <is>
-          <t>action_calculate_down_post</t>
-        </is>
-      </c>
-      <c r="E13" t="inlineStr"/>
+          <t>- action_deactivate_form</t>
+        </is>
+      </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr"/>
-      <c r="B14" t="inlineStr">
-        <is>
-          <t>cách tính chi tiết như nào thế</t>
-        </is>
-      </c>
+      <c r="B14" t="inlineStr"/>
       <c r="C14" t="inlineStr"/>
       <c r="D14" t="inlineStr">
         <is>
-          <t>request_more</t>
-        </is>
-      </c>
-      <c r="E14" t="inlineStr"/>
+          <t>- form{"name":null}</t>
+        </is>
+      </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr"/>
       <c r="B15" t="inlineStr"/>
-      <c r="C15" t="inlineStr">
-        <is>
-          <t>Xin lỗi, bot chỉ hỗ trợ bạn được như vậy thôi ạ!</t>
-        </is>
-      </c>
+      <c r="C15" t="inlineStr"/>
       <c r="D15" t="inlineStr">
         <is>
-          <t>utter_out_of_bot_ability</t>
-        </is>
-      </c>
-      <c r="E15" t="inlineStr"/>
+          <t>- slot{"requested_slot":null}</t>
+        </is>
+      </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr"/>
       <c r="B16" t="inlineStr"/>
-      <c r="C16" t="inlineStr">
-        <is>
-          <t>Trong trường hợp cần hỗ trợ, vui lòng liên hệ với bộ phận Chăm sóc khách hàng theo các kênh sau:
-• Gọi đến tổng đài theo số hotline 08.69.09.29.29
-• Gửi mail yêu cầu hỗ trợ tới địa chỉ “contact@meeyland.com”
-• Chat với "Chăm sóc khách hàng"</t>
-        </is>
-      </c>
+      <c r="C16" t="inlineStr"/>
       <c r="D16" t="inlineStr">
         <is>
-          <t>utter_how_contact_customer_service</t>
-        </is>
-      </c>
-      <c r="E16" t="inlineStr"/>
+          <t>- utter_confirm</t>
+        </is>
+      </c>
     </row>
     <row r="17">
-      <c r="A17" t="inlineStr">
-        <is>
-          <t>2</t>
-        </is>
-      </c>
-      <c r="B17" t="inlineStr">
-        <is>
-          <t>tôi muốn hạ tin hoàn tiền</t>
-        </is>
-      </c>
+      <c r="A17" t="inlineStr"/>
+      <c r="B17" t="inlineStr"/>
       <c r="C17" t="inlineStr"/>
       <c r="D17" t="inlineStr">
         <is>
-          <t>request_down_post</t>
-        </is>
-      </c>
-      <c r="E17" t="inlineStr"/>
+          <t>- utter_anything_else</t>
+        </is>
+      </c>
     </row>
     <row r="18">
-      <c r="A18" t="inlineStr"/>
-      <c r="B18" t="inlineStr"/>
-      <c r="C18" t="inlineStr">
-        <is>
-          <t>Bạn liên hệ bộ phận chăm sóc khách hàng để được hỗ trợ hạ tin và hoàn tiền về tài khoản nhé.
-Bot chỉ giúp bạn tính toán số tiền được hoàn trả khi hạ tin thôi ạ! Bạn vui lòng cung cấp một số thông tin.</t>
-        </is>
-      </c>
+      <c r="A18" t="inlineStr">
+        <is>
+          <t>4</t>
+        </is>
+      </c>
+      <c r="B18" t="inlineStr">
+        <is>
+          <t>Tôi muốn đổi gói tin</t>
+        </is>
+      </c>
+      <c r="C18" t="inlineStr"/>
       <c r="D18" t="inlineStr">
         <is>
-          <t>utter_bot_need_info_for_refund</t>
-        </is>
-      </c>
-      <c r="E18" t="inlineStr"/>
+          <t>* request_change_post_package</t>
+        </is>
+      </c>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr"/>
       <c r="B19" t="inlineStr"/>
-      <c r="C19" t="inlineStr">
-        <is>
-          <t>Bạn đang dùng gói vip nào</t>
-        </is>
-      </c>
+      <c r="C19" t="inlineStr"/>
       <c r="D19" t="inlineStr">
         <is>
-          <t>utter_ask_source_post_package</t>
-        </is>
-      </c>
-      <c r="E19" t="inlineStr"/>
+          <t>- utter_bot_need_info_for_change_source_package</t>
+        </is>
+      </c>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr"/>
-      <c r="B20" t="inlineStr">
-        <is>
-          <t>thôi ko cần đâu</t>
-        </is>
-      </c>
+      <c r="B20" t="inlineStr"/>
       <c r="C20" t="inlineStr"/>
       <c r="D20" t="inlineStr">
         <is>
-          <t>deny</t>
-        </is>
-      </c>
-      <c r="E20" t="inlineStr"/>
+          <t>- calculate_change_post_form</t>
+        </is>
+      </c>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr"/>
       <c r="B21" t="inlineStr"/>
-      <c r="C21" t="inlineStr">
-        <is>
-          <t>Vâng ạ</t>
-        </is>
-      </c>
+      <c r="C21" t="inlineStr"/>
       <c r="D21" t="inlineStr">
         <is>
-          <t>utter_confirm</t>
-        </is>
-      </c>
-      <c r="E21" t="inlineStr"/>
+          <t>- form{"name": "calculate_change_post_form"}</t>
+        </is>
+      </c>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr"/>
       <c r="B22" t="inlineStr"/>
-      <c r="C22" t="inlineStr">
-        <is>
-          <t>Bạn có thắc mắc hay cần giúp đỡ gì nữa không ạ</t>
-        </is>
-      </c>
+      <c r="C22" t="inlineStr"/>
       <c r="D22" t="inlineStr">
         <is>
-          <t>utter_anything_else</t>
-        </is>
-      </c>
-      <c r="E22" t="inlineStr"/>
+          <t xml:space="preserve">- form{"name": null} </t>
+        </is>
+      </c>
     </row>
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>3</t>
+          <t>5</t>
         </is>
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>tôi muốn hạ tin hoàn tiền</t>
+          <t>Tôi muốn đổi gói tin</t>
         </is>
       </c>
       <c r="C23" t="inlineStr"/>
       <c r="D23" t="inlineStr">
         <is>
-          <t>request_down_post</t>
-        </is>
-      </c>
-      <c r="E23" t="inlineStr"/>
+          <t>* request_change_post_package</t>
+        </is>
+      </c>
     </row>
     <row r="24">
       <c r="A24" t="inlineStr"/>
       <c r="B24" t="inlineStr"/>
-      <c r="C24" t="inlineStr">
-        <is>
-          <t>Bạn liên hệ bộ phận chăm sóc khách hàng để được hỗ trợ hạ tin và hoàn tiền về tài khoản nhé.
-Bot chỉ giúp bạn tính toán số tiền được hoàn trả khi hạ tin thôi ạ! Bạn vui lòng cung cấp một số thông tin.</t>
-        </is>
-      </c>
+      <c r="C24" t="inlineStr"/>
       <c r="D24" t="inlineStr">
         <is>
-          <t>utter_bot_need_info_for_refund</t>
-        </is>
-      </c>
-      <c r="E24" t="inlineStr"/>
+          <t>- utter_bot_need_info_for_change_source_package</t>
+        </is>
+      </c>
     </row>
     <row r="25">
       <c r="A25" t="inlineStr"/>
       <c r="B25" t="inlineStr"/>
-      <c r="C25" t="inlineStr">
-        <is>
-          <t>Bạn đang dùng gói vip nào</t>
-        </is>
-      </c>
+      <c r="C25" t="inlineStr"/>
       <c r="D25" t="inlineStr">
         <is>
-          <t>utter_ask_source_post_package</t>
-        </is>
-      </c>
-      <c r="E25" t="inlineStr"/>
+          <t>- calculate_change_post_form</t>
+        </is>
+      </c>
     </row>
     <row r="26">
       <c r="A26" t="inlineStr"/>
-      <c r="B26" t="inlineStr">
-        <is>
-          <t>bot làm giúp luôn đi</t>
-        </is>
-      </c>
+      <c r="B26" t="inlineStr"/>
       <c r="C26" t="inlineStr"/>
       <c r="D26" t="inlineStr">
         <is>
-          <t>request_more</t>
-        </is>
-      </c>
-      <c r="E26" t="inlineStr"/>
+          <t>- form{"name":"calculate_change_post_form"}</t>
+        </is>
+      </c>
     </row>
     <row r="27">
       <c r="A27" t="inlineStr"/>
       <c r="B27" t="inlineStr"/>
-      <c r="C27" t="inlineStr">
-        <is>
-          <t>Bạn liên hệ bộ phận chăm sóc khách hàng để được hỗ trợ hạ tin và hoàn tiền về tài khoản nhé.
-Bot chỉ giúp bạn tính toán số tiền được hoàn trả khi hạ tin thôi ạ! Bạn vui lòng cung cấp một số thông tin.</t>
-        </is>
-      </c>
+      <c r="C27" t="inlineStr"/>
       <c r="D27" t="inlineStr">
         <is>
-          <t>utter_bot_need_info_for_refund</t>
-        </is>
-      </c>
-      <c r="E27" t="inlineStr"/>
+          <t>- slot{"requested_slot":"source_post_package"}</t>
+        </is>
+      </c>
     </row>
     <row r="28">
       <c r="A28" t="inlineStr"/>
-      <c r="B28" t="inlineStr"/>
-      <c r="C28" t="inlineStr">
-        <is>
-          <t>Bạn đang dùng gói vip nào</t>
-        </is>
-      </c>
+      <c r="B28" t="inlineStr">
+        <is>
+          <t>Thế thôi ko cần đâu</t>
+        </is>
+      </c>
+      <c r="C28" t="inlineStr"/>
       <c r="D28" t="inlineStr">
         <is>
-          <t>utter_ask_source_post_package</t>
-        </is>
-      </c>
-      <c r="E28" t="inlineStr"/>
+          <t>* canthelp OR deny</t>
+        </is>
+      </c>
     </row>
     <row r="29">
-      <c r="A29" t="inlineStr">
-        <is>
-          <t>4</t>
-        </is>
-      </c>
-      <c r="B29" t="inlineStr">
-        <is>
-          <t>hạ tin hoàn tiền như nào</t>
-        </is>
-      </c>
+      <c r="A29" t="inlineStr"/>
+      <c r="B29" t="inlineStr"/>
       <c r="C29" t="inlineStr"/>
       <c r="D29" t="inlineStr">
         <is>
-          <t>request_down_post</t>
-        </is>
-      </c>
-      <c r="E29" t="inlineStr"/>
+          <t>- action_deactivate_form</t>
+        </is>
+      </c>
     </row>
     <row r="30">
       <c r="A30" t="inlineStr"/>
       <c r="B30" t="inlineStr"/>
-      <c r="C30" t="inlineStr">
-        <is>
-          <t>Bạn liên hệ bộ phận chăm sóc khách hàng để được hỗ trợ hạ tin và hoàn tiền về tài khoản nhé.
-Bot chỉ giúp bạn tính toán số tiền được hoàn trả khi hạ tin thôi ạ! Bạn vui lòng cung cấp một số thông tin.</t>
-        </is>
-      </c>
+      <c r="C30" t="inlineStr"/>
       <c r="D30" t="inlineStr">
         <is>
-          <t>utter_bot_need_info_for_refund</t>
-        </is>
-      </c>
-      <c r="E30" t="inlineStr"/>
+          <t>- form{"name":null}</t>
+        </is>
+      </c>
     </row>
     <row r="31">
       <c r="A31" t="inlineStr"/>
       <c r="B31" t="inlineStr"/>
-      <c r="C31" t="inlineStr">
-        <is>
-          <t>Bạn đang dùng gói vip nào</t>
-        </is>
-      </c>
+      <c r="C31" t="inlineStr"/>
       <c r="D31" t="inlineStr">
         <is>
-          <t>utter_ask_source_post_package</t>
-        </is>
-      </c>
-      <c r="E31" t="inlineStr"/>
+          <t>- slot{"requested_slot":null}</t>
+        </is>
+      </c>
     </row>
     <row r="32">
       <c r="A32" t="inlineStr"/>
-      <c r="B32" t="inlineStr">
-        <is>
-          <t>gói vip 3 nhé</t>
-        </is>
-      </c>
+      <c r="B32" t="inlineStr"/>
       <c r="C32" t="inlineStr"/>
       <c r="D32" t="inlineStr">
         <is>
-          <t>enter_data</t>
-        </is>
-      </c>
-      <c r="E32" t="inlineStr"/>
+          <t>- utter_confirm</t>
+        </is>
+      </c>
     </row>
     <row r="33">
       <c r="A33" t="inlineStr"/>
       <c r="B33" t="inlineStr"/>
-      <c r="C33" t="inlineStr">
-        <is>
-          <t>action_set_source_post_package</t>
-        </is>
-      </c>
+      <c r="C33" t="inlineStr"/>
       <c r="D33" t="inlineStr">
         <is>
-          <t>action_set_source_post_package</t>
-        </is>
-      </c>
-      <c r="E33" t="inlineStr"/>
-    </row>
-    <row r="34">
-      <c r="A34" t="inlineStr"/>
-      <c r="B34" t="inlineStr"/>
-      <c r="C34" t="inlineStr">
-        <is>
-          <t>Bạn mua gói vip trong bao nhiêu ngày?</t>
-        </is>
-      </c>
-      <c r="D34" t="inlineStr">
-        <is>
-          <t>utter_ask_buy_vip_duration</t>
-        </is>
-      </c>
-      <c r="E34" t="inlineStr"/>
-    </row>
-    <row r="35">
-      <c r="A35" t="inlineStr"/>
-      <c r="B35" t="inlineStr">
-        <is>
-          <t>29 ngày</t>
-        </is>
-      </c>
-      <c r="C35" t="inlineStr"/>
-      <c r="D35" t="inlineStr">
-        <is>
-          <t>enter_data</t>
-        </is>
-      </c>
-      <c r="E35" t="inlineStr"/>
-    </row>
-    <row r="36">
-      <c r="A36" t="inlineStr"/>
-      <c r="B36" t="inlineStr"/>
-      <c r="C36" t="inlineStr">
-        <is>
-          <t>action_set_buy_vip_duration</t>
-        </is>
-      </c>
-      <c r="D36" t="inlineStr">
-        <is>
-          <t>action_set_buy_vip_duration</t>
-        </is>
-      </c>
-      <c r="E36" t="inlineStr"/>
-    </row>
-    <row r="37">
-      <c r="A37" t="inlineStr"/>
-      <c r="B37" t="inlineStr"/>
-      <c r="C37" t="inlineStr">
-        <is>
-          <t>Số ngày mua gói tin không hợp lệ. 
-Hiện tại MeeyLand chỉ cung cấp các gói tin 1 ngày, 7 ngày, 15 ngày, 30 ngày và 90 ngày.
-Bạn vui lòng cung cấp lại số ngày bạn đã mua gói tin nhé!</t>
-        </is>
-      </c>
-      <c r="D37" t="inlineStr">
-        <is>
-          <t>utter_request_valid_buy_vip_duration</t>
-        </is>
-      </c>
-      <c r="E37" t="inlineStr"/>
-    </row>
-    <row r="38">
-      <c r="A38" t="inlineStr"/>
-      <c r="B38" t="inlineStr">
-        <is>
-          <t>à 30 ngày</t>
-        </is>
-      </c>
-      <c r="C38" t="inlineStr"/>
-      <c r="D38" t="inlineStr">
-        <is>
-          <t>enter_data</t>
-        </is>
-      </c>
-      <c r="E38" t="inlineStr"/>
-    </row>
-    <row r="39">
-      <c r="A39" t="inlineStr"/>
-      <c r="B39" t="inlineStr"/>
-      <c r="C39" t="inlineStr">
-        <is>
-          <t>action_set_buy_vip_duration</t>
-        </is>
-      </c>
-      <c r="D39" t="inlineStr">
-        <is>
-          <t>action_set_buy_vip_duration</t>
-        </is>
-      </c>
-      <c r="E39" t="inlineStr"/>
-    </row>
-    <row r="40">
-      <c r="A40" t="inlineStr"/>
-      <c r="B40" t="inlineStr"/>
-      <c r="C40" t="inlineStr">
-        <is>
-          <t>Bạn đã sử dụng trong bao ngày rồi?</t>
-        </is>
-      </c>
-      <c r="D40" t="inlineStr">
-        <is>
-          <t>utter_ask_used_vip_duration</t>
-        </is>
-      </c>
-      <c r="E40" t="inlineStr"/>
-    </row>
-    <row r="41">
-      <c r="A41" t="inlineStr"/>
-      <c r="B41" t="inlineStr">
-        <is>
-          <t>17 ngày rồi</t>
-        </is>
-      </c>
-      <c r="C41" t="inlineStr"/>
-      <c r="D41" t="inlineStr">
-        <is>
-          <t>enter_data</t>
-        </is>
-      </c>
-      <c r="E41" t="inlineStr"/>
-    </row>
-    <row r="42">
-      <c r="A42" t="inlineStr"/>
-      <c r="B42" t="inlineStr"/>
-      <c r="C42" t="inlineStr">
-        <is>
-          <t>action_set_used_vip_duration</t>
-        </is>
-      </c>
-      <c r="D42" t="inlineStr">
-        <is>
-          <t>action_set_used_vip_duration</t>
-        </is>
-      </c>
-      <c r="E42" t="inlineStr"/>
-    </row>
-    <row r="43">
-      <c r="A43" t="inlineStr"/>
-      <c r="B43" t="inlineStr"/>
-      <c r="C43" t="inlineStr">
-        <is>
-          <t>action_calculate_down_post</t>
-        </is>
-      </c>
-      <c r="D43" t="inlineStr">
-        <is>
-          <t>action_calculate_down_post</t>
-        </is>
-      </c>
-      <c r="E43" t="inlineStr"/>
-    </row>
-    <row r="44">
-      <c r="A44" t="inlineStr"/>
-      <c r="B44" t="inlineStr">
-        <is>
-          <t>cách tính chi tiết như nào thế</t>
-        </is>
-      </c>
-      <c r="C44" t="inlineStr"/>
-      <c r="D44" t="inlineStr">
-        <is>
-          <t>request_more</t>
-        </is>
-      </c>
-      <c r="E44" t="inlineStr"/>
-    </row>
-    <row r="45">
-      <c r="A45" t="inlineStr"/>
-      <c r="B45" t="inlineStr"/>
-      <c r="C45" t="inlineStr">
-        <is>
-          <t>Xin lỗi, bot chỉ hỗ trợ bạn được như vậy thôi ạ!</t>
-        </is>
-      </c>
-      <c r="D45" t="inlineStr">
-        <is>
-          <t>utter_out_of_bot_ability</t>
-        </is>
-      </c>
-      <c r="E45" t="inlineStr"/>
-    </row>
-    <row r="46">
-      <c r="A46" t="inlineStr"/>
-      <c r="B46" t="inlineStr"/>
-      <c r="C46" t="inlineStr">
-        <is>
-          <t>Bạn liên hệ để được hỗ trợ nâng cao:
-• Gọi đến tổng đài theo số hotline 08.69.09.29.29
-• Gửi mail yêu cầu hỗ trợ tới địa chỉ “contact@meeyland.com”
-• Chat với "Chăm sóc khách hàng"</t>
-        </is>
-      </c>
-      <c r="D46" t="inlineStr">
-        <is>
-          <t>utter_how_contact_customer_service</t>
-        </is>
-      </c>
-      <c r="E46" t="inlineStr"/>
-    </row>
-    <row r="47">
-      <c r="A47" t="inlineStr">
-        <is>
-          <t>5</t>
-        </is>
-      </c>
-      <c r="B47" t="inlineStr">
-        <is>
-          <t>hoàn tiền không khi tôi hạ tin</t>
-        </is>
-      </c>
-      <c r="C47" t="inlineStr"/>
-      <c r="D47" t="inlineStr">
-        <is>
-          <t>is_refund_after_putdown_post</t>
-        </is>
-      </c>
-      <c r="E47" t="inlineStr"/>
-    </row>
-    <row r="48">
-      <c r="A48" t="inlineStr"/>
-      <c r="B48" t="inlineStr"/>
-      <c r="C48" t="inlineStr">
-        <is>
-          <t>Chính sách của MeeyLand hiện tại cho phép hoàn tiền một phần/toàn bộ, tùy theo chính sách của MeeyLand từng thời kỳ bạn nhé!</t>
-        </is>
-      </c>
-      <c r="D48" t="inlineStr">
-        <is>
-          <t>utter_is_refund_after_putdown_post</t>
-        </is>
-      </c>
-      <c r="E48" t="inlineStr"/>
-    </row>
-    <row r="49">
-      <c r="A49" t="inlineStr"/>
-      <c r="B49" t="inlineStr"/>
-      <c r="C49" t="inlineStr">
-        <is>
-          <t>Bạn liên hệ bộ phận chăm sóc khách hàng để được hỗ trợ hạ tin và hoàn tiền về tài khoản nhé.
-Bot chỉ giúp bạn tính toán số tiền được hoàn trả khi hạ tin thôi ạ! Bạn vui lòng cung cấp một số thông tin.</t>
-        </is>
-      </c>
-      <c r="D49" t="inlineStr">
-        <is>
-          <t>utter_bot_need_info_for_refund</t>
-        </is>
-      </c>
-      <c r="E49" t="inlineStr"/>
-    </row>
-    <row r="50">
-      <c r="A50" t="inlineStr"/>
-      <c r="B50" t="inlineStr"/>
-      <c r="C50" t="inlineStr">
-        <is>
-          <t>Bạn đang dùng gói vip nào</t>
-        </is>
-      </c>
-      <c r="D50" t="inlineStr">
-        <is>
-          <t>utter_ask_source_post_package</t>
-        </is>
-      </c>
-      <c r="E50" t="inlineStr"/>
-    </row>
-    <row r="51">
-      <c r="A51" t="inlineStr"/>
-      <c r="B51" t="inlineStr">
-        <is>
-          <t>gói vip 3</t>
-        </is>
-      </c>
-      <c r="C51" t="inlineStr"/>
-      <c r="D51" t="inlineStr">
-        <is>
-          <t>enter_data</t>
-        </is>
-      </c>
-      <c r="E51" t="inlineStr"/>
-    </row>
-    <row r="52">
-      <c r="A52" t="inlineStr"/>
-      <c r="B52" t="inlineStr"/>
-      <c r="C52" t="inlineStr">
-        <is>
-          <t>action_set_source_post_package</t>
-        </is>
-      </c>
-      <c r="D52" t="inlineStr">
-        <is>
-          <t>action_set_source_post_package</t>
-        </is>
-      </c>
-      <c r="E52" t="inlineStr"/>
-    </row>
-    <row r="53">
-      <c r="A53" t="inlineStr"/>
-      <c r="B53" t="inlineStr"/>
-      <c r="C53" t="inlineStr">
-        <is>
-          <t>Số ngày mua ban đầu là bao nhiêu?</t>
-        </is>
-      </c>
-      <c r="D53" t="inlineStr">
-        <is>
-          <t>utter_ask_buy_vip_duration</t>
-        </is>
-      </c>
-      <c r="E53" t="inlineStr"/>
-    </row>
-    <row r="54">
-      <c r="A54" t="inlineStr"/>
-      <c r="B54" t="inlineStr">
-        <is>
-          <t>Mình mua 15 ngày</t>
-        </is>
-      </c>
-      <c r="C54" t="inlineStr"/>
-      <c r="D54" t="inlineStr">
-        <is>
-          <t>enter_data</t>
-        </is>
-      </c>
-      <c r="E54" t="inlineStr"/>
-    </row>
-    <row r="55">
-      <c r="A55" t="inlineStr"/>
-      <c r="B55" t="inlineStr"/>
-      <c r="C55" t="inlineStr">
-        <is>
-          <t>action_set_buy_vip_duration</t>
-        </is>
-      </c>
-      <c r="D55" t="inlineStr">
-        <is>
-          <t>action_set_buy_vip_duration</t>
-        </is>
-      </c>
-      <c r="E55" t="inlineStr"/>
-    </row>
-    <row r="56">
-      <c r="A56" t="inlineStr"/>
-      <c r="B56" t="inlineStr"/>
-      <c r="C56" t="inlineStr">
-        <is>
-          <t>Bạn đã sử dụng trong bao ngày rồi?</t>
-        </is>
-      </c>
-      <c r="D56" t="inlineStr">
-        <is>
-          <t>utter_ask_used_vip_duration</t>
-        </is>
-      </c>
-      <c r="E56" t="inlineStr"/>
-    </row>
-    <row r="57">
-      <c r="A57" t="inlineStr"/>
-      <c r="B57" t="inlineStr">
-        <is>
-          <t>mời dùng có 3 ngày thôi</t>
-        </is>
-      </c>
-      <c r="C57" t="inlineStr"/>
-      <c r="D57" t="inlineStr">
-        <is>
-          <t>enter_data</t>
-        </is>
-      </c>
-      <c r="E57" t="inlineStr"/>
-    </row>
-    <row r="58">
-      <c r="A58" t="inlineStr"/>
-      <c r="B58" t="inlineStr"/>
-      <c r="C58" t="inlineStr">
-        <is>
-          <t>action_set_used_vip_duration</t>
-        </is>
-      </c>
-      <c r="D58" t="inlineStr">
-        <is>
-          <t>action_set_used_vip_duration</t>
-        </is>
-      </c>
-      <c r="E58" t="inlineStr"/>
-    </row>
-    <row r="59">
-      <c r="A59" t="inlineStr"/>
-      <c r="B59" t="inlineStr"/>
-      <c r="C59" t="inlineStr">
-        <is>
-          <t>Số tiền bạn được hoàn trả là ...</t>
-        </is>
-      </c>
-      <c r="D59" t="inlineStr">
-        <is>
-          <t>action_calculate_down_post</t>
-        </is>
-      </c>
-      <c r="E59" t="inlineStr"/>
-    </row>
-    <row r="60">
-      <c r="A60" t="inlineStr"/>
-      <c r="B60" t="inlineStr">
-        <is>
-          <t>cách tính chi tiết như nào thế</t>
-        </is>
-      </c>
-      <c r="C60" t="inlineStr"/>
-      <c r="D60" t="inlineStr">
-        <is>
-          <t>request_more</t>
-        </is>
-      </c>
-      <c r="E60" t="inlineStr"/>
-    </row>
-    <row r="61">
-      <c r="A61" t="inlineStr"/>
-      <c r="B61" t="inlineStr"/>
-      <c r="C61" t="inlineStr">
-        <is>
-          <t>Xin lỗi, bot chỉ hỗ trợ bạn được như vậy thôi ạ!</t>
-        </is>
-      </c>
-      <c r="D61" t="inlineStr">
-        <is>
-          <t>utter_out_of_bot_ability</t>
-        </is>
-      </c>
-      <c r="E61" t="inlineStr"/>
-    </row>
-    <row r="62">
-      <c r="A62" t="inlineStr"/>
-      <c r="B62" t="inlineStr"/>
-      <c r="C62" t="inlineStr">
-        <is>
-          <t>Bạn liên hệ để được hỗ trợ nâng cao:
-• Gọi đến tổng đài theo số hotline 08.69.09.29.29
-• Gửi mail yêu cầu hỗ trợ tới địa chỉ “contact@meeyland.com”
-• Chat với "Chăm sóc khách hàng"</t>
-        </is>
-      </c>
-      <c r="D62" t="inlineStr">
-        <is>
-          <t>utter_how_contact_customer_service</t>
-        </is>
-      </c>
-      <c r="E62" t="inlineStr"/>
-    </row>
-    <row r="63">
-      <c r="A63" t="inlineStr">
-        <is>
-          <t>6</t>
-        </is>
-      </c>
-      <c r="B63" t="inlineStr">
-        <is>
-          <t>hoàn tiền không khi tôi hạ tin</t>
-        </is>
-      </c>
-      <c r="C63" t="inlineStr"/>
-      <c r="D63" t="inlineStr">
-        <is>
-          <t>is_refund_after_putdown_post</t>
-        </is>
-      </c>
-      <c r="E63" t="inlineStr"/>
-    </row>
-    <row r="64">
-      <c r="A64" t="inlineStr"/>
-      <c r="B64" t="inlineStr"/>
-      <c r="C64" t="inlineStr">
-        <is>
-          <t>Chính sách của MeeyLand hiện tại cho phép hoàn tiền một phần/toàn bộ, tùy theo chính sách của MeeyLand từng thời kỳ bạn nhé!</t>
-        </is>
-      </c>
-      <c r="D64" t="inlineStr">
-        <is>
-          <t>utter_is_refund_after_putdown_post</t>
-        </is>
-      </c>
-      <c r="E64" t="inlineStr"/>
-    </row>
-    <row r="65">
-      <c r="A65" t="inlineStr"/>
-      <c r="B65" t="inlineStr"/>
-      <c r="C65" t="inlineStr">
-        <is>
-          <t>Bạn liên hệ bộ phận chăm sóc khách hàng để được hỗ trợ hạ tin và hoàn tiền về tài khoản nhé.
-Bot chỉ giúp bạn tính toán số tiền được hoàn trả khi hạ tin thôi ạ! Bạn vui lòng cung cấp một số thông tin.</t>
-        </is>
-      </c>
-      <c r="D65" t="inlineStr">
-        <is>
-          <t>utter_bot_need_info_for_refund</t>
-        </is>
-      </c>
-      <c r="E65" t="inlineStr"/>
-    </row>
-    <row r="66">
-      <c r="A66" t="inlineStr"/>
-      <c r="B66" t="inlineStr"/>
-      <c r="C66" t="inlineStr">
-        <is>
-          <t>Bạn đang dùng gói vip nào</t>
-        </is>
-      </c>
-      <c r="D66" t="inlineStr">
-        <is>
-          <t>utter_ask_source_post_package</t>
-        </is>
-      </c>
-      <c r="E66" t="inlineStr"/>
-    </row>
-    <row r="67">
-      <c r="A67" t="inlineStr"/>
-      <c r="B67" t="inlineStr">
-        <is>
-          <t>thôi ko cần đâu</t>
-        </is>
-      </c>
-      <c r="C67" t="inlineStr"/>
-      <c r="D67" t="inlineStr">
-        <is>
-          <t>deny</t>
-        </is>
-      </c>
-      <c r="E67" t="inlineStr"/>
-    </row>
-    <row r="68">
-      <c r="A68" t="inlineStr"/>
-      <c r="B68" t="inlineStr"/>
-      <c r="C68" t="inlineStr">
-        <is>
-          <t>Vâng ạ</t>
-        </is>
-      </c>
-      <c r="D68" t="inlineStr">
-        <is>
-          <t>utter_confirm</t>
-        </is>
-      </c>
-      <c r="E68" t="inlineStr"/>
-    </row>
-    <row r="69">
-      <c r="A69" t="inlineStr"/>
-      <c r="B69" t="inlineStr"/>
-      <c r="C69" t="inlineStr">
-        <is>
-          <t>Bạn có thắc mắc hay cần giúp đỡ gì nữa không ạ</t>
-        </is>
-      </c>
-      <c r="D69" t="inlineStr">
-        <is>
-          <t>utter_anything_else</t>
-        </is>
-      </c>
-      <c r="E69" t="inlineStr"/>
-    </row>
-    <row r="70">
-      <c r="A70" t="inlineStr">
-        <is>
-          <t>7</t>
-        </is>
-      </c>
-      <c r="B70" t="inlineStr">
-        <is>
-          <t>hoàn tiền không khi tôi hạ tin</t>
-        </is>
-      </c>
-      <c r="C70" t="inlineStr"/>
-      <c r="D70" t="inlineStr">
-        <is>
-          <t>is_refund_after_putdown_post</t>
-        </is>
-      </c>
-      <c r="E70" t="inlineStr"/>
-    </row>
-    <row r="71">
-      <c r="A71" t="inlineStr"/>
-      <c r="B71" t="inlineStr"/>
-      <c r="C71" t="inlineStr">
-        <is>
-          <t>Chính sách của MeeyLand hiện tại cho phép hoàn tiền một phần/toàn bộ, tùy theo chính sách của MeeyLand từng thời kỳ bạn nhé!</t>
-        </is>
-      </c>
-      <c r="D71" t="inlineStr">
-        <is>
-          <t>utter_is_refund_after_putdown_post</t>
-        </is>
-      </c>
-      <c r="E71" t="inlineStr"/>
-    </row>
-    <row r="72">
-      <c r="A72" t="inlineStr"/>
-      <c r="B72" t="inlineStr"/>
-      <c r="C72" t="inlineStr">
-        <is>
-          <t>Bạn liên hệ bộ phận chăm sóc khách hàng để được hỗ trợ hạ tin và hoàn tiền về tài khoản nhé.
-Bot chỉ giúp bạn tính toán số tiền được hoàn trả khi hạ tin thôi ạ! Bạn vui lòng cung cấp một số thông tin.</t>
-        </is>
-      </c>
-      <c r="D72" t="inlineStr">
-        <is>
-          <t>utter_bot_need_info_for_refund</t>
-        </is>
-      </c>
-      <c r="E72" t="inlineStr"/>
-    </row>
-    <row r="73">
-      <c r="A73" t="inlineStr"/>
-      <c r="B73" t="inlineStr"/>
-      <c r="C73" t="inlineStr">
-        <is>
-          <t>Bạn đang dùng gói vip nào</t>
-        </is>
-      </c>
-      <c r="D73" t="inlineStr">
-        <is>
-          <t>utter_ask_source_post_package</t>
-        </is>
-      </c>
-      <c r="E73" t="inlineStr"/>
-    </row>
-    <row r="74">
-      <c r="A74" t="inlineStr"/>
-      <c r="B74" t="inlineStr">
-        <is>
-          <t>bot làm giúp luôn đi</t>
-        </is>
-      </c>
-      <c r="C74" t="inlineStr"/>
-      <c r="D74" t="inlineStr">
-        <is>
-          <t>request_more</t>
-        </is>
-      </c>
-      <c r="E74" t="inlineStr"/>
-    </row>
-    <row r="75">
-      <c r="A75" t="inlineStr"/>
-      <c r="B75" t="inlineStr"/>
-      <c r="C75" t="inlineStr">
-        <is>
-          <t>Bạn liên hệ bộ phận chăm sóc khách hàng để được hỗ trợ hạ tin và hoàn tiền về tài khoản nhé.
-Bot chỉ giúp bạn tính toán số tiền được hoàn trả khi hạ tin thôi ạ! Bạn vui lòng cung cấp một số thông tin.</t>
-        </is>
-      </c>
-      <c r="D75" t="inlineStr">
-        <is>
-          <t>utter_bot_need_info_for_refund</t>
-        </is>
-      </c>
-      <c r="E75" t="inlineStr"/>
-    </row>
-    <row r="76">
-      <c r="A76" t="inlineStr"/>
-      <c r="B76" t="inlineStr"/>
-      <c r="C76" t="inlineStr">
-        <is>
-          <t>Bạn đang dùng gói vip nào</t>
-        </is>
-      </c>
-      <c r="D76" t="inlineStr">
-        <is>
-          <t>utter_ask_source_post_package</t>
-        </is>
-      </c>
-      <c r="E76" t="inlineStr"/>
-    </row>
-    <row r="77">
-      <c r="A77" t="inlineStr">
-        <is>
-          <t>8</t>
-        </is>
-      </c>
-      <c r="B77" t="inlineStr">
-        <is>
-          <t>Hạn tin hoàn tiền</t>
-        </is>
-      </c>
-      <c r="C77" t="inlineStr"/>
-      <c r="D77" t="inlineStr">
-        <is>
-          <t>request_down_post</t>
-        </is>
-      </c>
-      <c r="E77" t="inlineStr"/>
-    </row>
-    <row r="78">
-      <c r="A78" t="inlineStr"/>
-      <c r="B78" t="inlineStr"/>
-      <c r="C78" t="inlineStr">
-        <is>
-          <t>Bạn liên hệ bộ phận chăm sóc khách hàng để được hỗ trợ hạ tin và hoàn tiền về tài khoản nhé.
-Bot chỉ giúp bạn tính toán số tiền được hoàn trả khi hạ tin thôi ạ! Bạn vui lòng cung cấp một số thông tin.</t>
-        </is>
-      </c>
-      <c r="D78" t="inlineStr">
-        <is>
-          <t>utter_bot_need_info_for_refund</t>
-        </is>
-      </c>
-      <c r="E78" t="inlineStr"/>
-    </row>
-    <row r="79">
-      <c r="A79" t="inlineStr"/>
-      <c r="B79" t="inlineStr"/>
-      <c r="C79" t="inlineStr">
-        <is>
-          <t>Bạn dùng gói vip nào</t>
-        </is>
-      </c>
-      <c r="D79" t="inlineStr">
-        <is>
-          <t>utter_ask_source_post_package</t>
-        </is>
-      </c>
-      <c r="E79" t="inlineStr"/>
-    </row>
-    <row r="80">
-      <c r="A80" t="inlineStr"/>
-      <c r="B80" t="inlineStr">
-        <is>
-          <t>vip 3 nhé</t>
-        </is>
-      </c>
-      <c r="C80" t="inlineStr"/>
-      <c r="D80" t="inlineStr">
-        <is>
-          <t>enter_data{"post_package":"vip 3"}</t>
-        </is>
-      </c>
-      <c r="E80" t="inlineStr"/>
-    </row>
-    <row r="81">
-      <c r="A81" t="inlineStr"/>
-      <c r="B81" t="inlineStr"/>
-      <c r="C81" t="inlineStr">
-        <is>
-          <t>bot</t>
-        </is>
-      </c>
-      <c r="D81" t="inlineStr">
-        <is>
-          <t>slot{"post_package":"vip 3"}</t>
-        </is>
-      </c>
-      <c r="E81" t="inlineStr"/>
-    </row>
-    <row r="82">
-      <c r="A82" t="inlineStr"/>
-      <c r="B82" t="inlineStr"/>
-      <c r="C82" t="inlineStr">
-        <is>
-          <t>set buy slot</t>
-        </is>
-      </c>
-      <c r="D82" t="inlineStr">
-        <is>
-          <t>action_set_source_post_package</t>
-        </is>
-      </c>
-      <c r="E82" t="inlineStr"/>
-    </row>
-    <row r="83">
-      <c r="A83" t="inlineStr"/>
-      <c r="B83" t="inlineStr"/>
-      <c r="C83" t="inlineStr">
-        <is>
-          <t>bot</t>
-        </is>
-      </c>
-      <c r="D83" t="inlineStr">
-        <is>
-          <t>slot{"source_post_package":"vip 3"}</t>
-        </is>
-      </c>
-      <c r="E83" t="inlineStr"/>
-    </row>
-    <row r="84">
-      <c r="A84" t="inlineStr"/>
-      <c r="B84" t="inlineStr"/>
-      <c r="C84" t="inlineStr">
-        <is>
-          <t>bot</t>
-        </is>
-      </c>
-      <c r="D84" t="inlineStr">
-        <is>
-          <t>slot{"post_package":"None"}</t>
-        </is>
-      </c>
-      <c r="E84" t="inlineStr"/>
-    </row>
-    <row r="85">
-      <c r="A85" t="inlineStr"/>
-      <c r="B85" t="inlineStr"/>
-      <c r="C85" t="inlineStr">
-        <is>
-          <t>Số ngày mua ban đầu là bao nhiêu</t>
-        </is>
-      </c>
-      <c r="D85" t="inlineStr">
-        <is>
-          <t>utter_ask_buy_vip_duration</t>
-        </is>
-      </c>
-      <c r="E85" t="inlineStr"/>
-    </row>
-    <row r="86">
-      <c r="A86" t="inlineStr"/>
-      <c r="B86" t="inlineStr">
-        <is>
-          <t>30 ngày nhé</t>
-        </is>
-      </c>
-      <c r="C86" t="inlineStr"/>
-      <c r="D86" t="inlineStr">
-        <is>
-          <t>enter_data{"duration":"30 ngày"}</t>
-        </is>
-      </c>
-      <c r="E86" t="inlineStr"/>
-    </row>
-    <row r="87">
-      <c r="A87" t="inlineStr"/>
-      <c r="B87" t="inlineStr"/>
-      <c r="C87" t="inlineStr">
-        <is>
-          <t>bot</t>
-        </is>
-      </c>
-      <c r="D87" t="inlineStr">
-        <is>
-          <t>slot{"duration":"30 ngày"}</t>
-        </is>
-      </c>
-      <c r="E87" t="inlineStr"/>
-    </row>
-    <row r="88">
-      <c r="A88" t="inlineStr"/>
-      <c r="B88" t="inlineStr"/>
-      <c r="C88" t="inlineStr">
-        <is>
-          <t>action set</t>
-        </is>
-      </c>
-      <c r="D88" t="inlineStr">
-        <is>
-          <t>action_set_buy_vip_duration</t>
-        </is>
-      </c>
-      <c r="E88" t="inlineStr"/>
-    </row>
-    <row r="89">
-      <c r="A89" t="inlineStr"/>
-      <c r="B89" t="inlineStr"/>
-      <c r="C89" t="inlineStr">
-        <is>
-          <t>bot</t>
-        </is>
-      </c>
-      <c r="D89" t="inlineStr">
-        <is>
-          <t>slot{"buy_vip_duration":"30 ngày"}</t>
-        </is>
-      </c>
-      <c r="E89" t="inlineStr"/>
-    </row>
-    <row r="90">
-      <c r="A90" t="inlineStr"/>
-      <c r="B90" t="inlineStr"/>
-      <c r="C90" t="inlineStr">
-        <is>
-          <t>bot</t>
-        </is>
-      </c>
-      <c r="D90" t="inlineStr">
-        <is>
-          <t>slot{"duration":"None"}</t>
-        </is>
-      </c>
-      <c r="E90" t="inlineStr"/>
-    </row>
-    <row r="91">
-      <c r="A91" t="inlineStr"/>
-      <c r="B91" t="inlineStr"/>
-      <c r="C91" t="inlineStr">
-        <is>
-          <t>Bạn đã dùng trong bao lâu</t>
-        </is>
-      </c>
-      <c r="D91" t="inlineStr">
-        <is>
-          <t>utter_ask_used_vip_duration</t>
-        </is>
-      </c>
-      <c r="E91" t="inlineStr"/>
-    </row>
-    <row r="92">
-      <c r="A92" t="inlineStr"/>
-      <c r="B92" t="inlineStr">
-        <is>
-          <t>9 ngày rồi</t>
-        </is>
-      </c>
-      <c r="C92" t="inlineStr"/>
-      <c r="D92" t="inlineStr">
-        <is>
-          <t>enter_data{"duration":"9 ngày"}</t>
-        </is>
-      </c>
-      <c r="E92" t="inlineStr"/>
-    </row>
-    <row r="93">
-      <c r="A93" t="inlineStr"/>
-      <c r="B93" t="inlineStr"/>
-      <c r="C93" t="inlineStr">
-        <is>
-          <t>bot</t>
-        </is>
-      </c>
-      <c r="D93" t="inlineStr">
-        <is>
-          <t>slot{"duration":"9 ngày"}</t>
-        </is>
-      </c>
-      <c r="E93" t="inlineStr"/>
-    </row>
-    <row r="94">
-      <c r="A94" t="inlineStr"/>
-      <c r="B94" t="inlineStr"/>
-      <c r="C94" t="inlineStr">
-        <is>
-          <t>action set</t>
-        </is>
-      </c>
-      <c r="D94" t="inlineStr">
-        <is>
-          <t>action_set_used_vip_duration</t>
-        </is>
-      </c>
-      <c r="E94" t="inlineStr"/>
-    </row>
-    <row r="95">
-      <c r="A95" t="inlineStr"/>
-      <c r="B95" t="inlineStr"/>
-      <c r="C95" t="inlineStr">
-        <is>
-          <t>bot</t>
-        </is>
-      </c>
-      <c r="D95" t="inlineStr">
-        <is>
-          <t>slot{"used_vip_duration":"9 ngày"}</t>
-        </is>
-      </c>
-      <c r="E95" t="inlineStr"/>
-    </row>
-    <row r="96">
-      <c r="A96" t="inlineStr"/>
-      <c r="B96" t="inlineStr"/>
-      <c r="C96" t="inlineStr">
-        <is>
-          <t>bot</t>
-        </is>
-      </c>
-      <c r="D96" t="inlineStr">
-        <is>
-          <t>slot{"duration":"None"}</t>
-        </is>
-      </c>
-      <c r="E96" t="inlineStr"/>
-    </row>
-    <row r="97">
-      <c r="A97" t="inlineStr"/>
-      <c r="B97" t="inlineStr"/>
-      <c r="C97" t="inlineStr">
-        <is>
-          <t>action utter</t>
-        </is>
-      </c>
-      <c r="D97" t="inlineStr">
-        <is>
-          <t>action_calculate_down_post</t>
-        </is>
-      </c>
-      <c r="E97" t="inlineStr"/>
-    </row>
-    <row r="98">
-      <c r="A98" t="inlineStr"/>
-      <c r="B98" t="inlineStr">
-        <is>
-          <t>cách tính chi tiết như nào thế</t>
-        </is>
-      </c>
-      <c r="C98" t="inlineStr"/>
-      <c r="D98" t="inlineStr">
-        <is>
-          <t>request_more</t>
-        </is>
-      </c>
-      <c r="E98" t="inlineStr"/>
-    </row>
-    <row r="99">
-      <c r="A99" t="inlineStr"/>
-      <c r="B99" t="inlineStr"/>
-      <c r="C99" t="inlineStr">
-        <is>
-          <t>Xin lỗi, bot chỉ hỗ trợ bạn được như vậy thôi ạ!</t>
-        </is>
-      </c>
-      <c r="D99" t="inlineStr">
-        <is>
-          <t>utter_out_of_bot_ability</t>
-        </is>
-      </c>
-      <c r="E99" t="inlineStr"/>
-    </row>
-    <row r="100">
-      <c r="A100" t="inlineStr"/>
-      <c r="B100" t="inlineStr"/>
-      <c r="C100" t="inlineStr">
-        <is>
-          <t>Bạn liên hệ để được hỗ trợ nâng cao:
-• Gọi đến tổng đài theo số hotline 08.69.09.29.29
-• Gửi mail yêu cầu hỗ trợ tới địa chỉ “contact@meeyland.com”
-• Chat với "Chăm sóc khách hàng"</t>
-        </is>
-      </c>
-      <c r="D100" t="inlineStr">
-        <is>
-          <t>utter_how_contact_customer_service</t>
-        </is>
-      </c>
-      <c r="E100" t="inlineStr"/>
-    </row>
-    <row r="101">
-      <c r="A101" t="inlineStr">
-        <is>
-          <t>9</t>
-        </is>
-      </c>
-      <c r="B101" t="inlineStr">
-        <is>
-          <t>hạ tin hoàn tiền</t>
-        </is>
-      </c>
-      <c r="C101" t="inlineStr"/>
-      <c r="D101" t="inlineStr">
-        <is>
-          <t>request_down_post</t>
-        </is>
-      </c>
-      <c r="E101" t="inlineStr">
-        <is>
-          <t>* request_down_post</t>
-        </is>
-      </c>
-    </row>
-    <row r="102">
-      <c r="A102" t="inlineStr"/>
-      <c r="B102" t="inlineStr"/>
-      <c r="C102" t="inlineStr">
-        <is>
-          <t>Bạn liên hệ bộ phận chăm sóc khách hàng để được hỗ trợ hạ tin và hoàn tiền về tài khoản nhé.
-Bot chỉ giúp bạn tính toán số tiền được hoàn trả khi hạ tin thôi ạ! Bạn vui lòng cung cấp một số thông tin.</t>
-        </is>
-      </c>
-      <c r="D102" t="inlineStr">
-        <is>
-          <t>utter_bot_need_info_for_refund</t>
-        </is>
-      </c>
-      <c r="E102" t="inlineStr">
-        <is>
-          <t>- utter_bot_need_info_for_refund</t>
-        </is>
-      </c>
-    </row>
-    <row r="103">
-      <c r="A103" t="inlineStr"/>
-      <c r="B103" t="inlineStr"/>
-      <c r="C103" t="inlineStr">
-        <is>
-          <t>Bạn đang dùng vip mấy</t>
-        </is>
-      </c>
-      <c r="D103" t="inlineStr">
-        <is>
-          <t>utter_ask_source_post_package</t>
-        </is>
-      </c>
-      <c r="E103" t="inlineStr">
-        <is>
-          <t>- utter_ask_source_post_package</t>
-        </is>
-      </c>
-    </row>
-    <row r="104">
-      <c r="A104" t="inlineStr"/>
-      <c r="B104" t="inlineStr">
-        <is>
-          <t>gói vip 1 nhé</t>
-        </is>
-      </c>
-      <c r="C104" t="inlineStr"/>
-      <c r="D104" t="inlineStr">
-        <is>
-          <t>enter_data{"post_package":"vip 1"}</t>
-        </is>
-      </c>
-      <c r="E104" t="inlineStr">
-        <is>
-          <t>* enter_data{"post_package":"vip 3"}</t>
-        </is>
-      </c>
-    </row>
-    <row r="105">
-      <c r="A105" t="inlineStr"/>
-      <c r="B105" t="inlineStr"/>
-      <c r="C105" t="inlineStr">
-        <is>
-          <t>slot</t>
-        </is>
-      </c>
-      <c r="D105" t="inlineStr">
-        <is>
-          <t>slot{"post_package":"vip 1"}</t>
-        </is>
-      </c>
-      <c r="E105" t="inlineStr">
-        <is>
-          <t>- slot{"post_package":"vip 3"}</t>
-        </is>
-      </c>
-    </row>
-    <row r="106">
-      <c r="A106" t="inlineStr"/>
-      <c r="B106" t="inlineStr"/>
-      <c r="C106" t="inlineStr">
-        <is>
-          <t>set_post_package</t>
-        </is>
-      </c>
-      <c r="D106" t="inlineStr">
-        <is>
-          <t>action_set_source_post_package</t>
-        </is>
-      </c>
-      <c r="E106" t="inlineStr">
-        <is>
-          <t>- action_set_source_post_package</t>
-        </is>
-      </c>
-    </row>
-    <row r="107">
-      <c r="A107" t="inlineStr"/>
-      <c r="B107" t="inlineStr"/>
-      <c r="C107" t="inlineStr">
-        <is>
-          <t>slot</t>
-        </is>
-      </c>
-      <c r="D107" t="inlineStr">
-        <is>
-          <t>slot{"source_post_package":"vip 1"}</t>
-        </is>
-      </c>
-      <c r="E107" t="inlineStr">
-        <is>
-          <t>- slot{"source_post_package":"vip 3"}</t>
-        </is>
-      </c>
-    </row>
-    <row r="108">
-      <c r="A108" t="inlineStr"/>
-      <c r="B108" t="inlineStr"/>
-      <c r="C108" t="inlineStr">
-        <is>
-          <t>slot</t>
-        </is>
-      </c>
-      <c r="D108" t="inlineStr">
-        <is>
-          <t>slot{"post_package":"None"}</t>
-        </is>
-      </c>
-      <c r="E108" t="inlineStr">
-        <is>
-          <t>- slot{"post_package":"None"}</t>
-        </is>
-      </c>
-    </row>
-    <row r="109">
-      <c r="A109" t="inlineStr"/>
-      <c r="B109" t="inlineStr"/>
-      <c r="C109" t="inlineStr">
-        <is>
-          <t>Số ngày ban đầu bạn đã mua?</t>
-        </is>
-      </c>
-      <c r="D109" t="inlineStr">
-        <is>
-          <t>utter_ask_buy_vip_duration</t>
-        </is>
-      </c>
-      <c r="E109" t="inlineStr">
-        <is>
-          <t>- utter_ask_buy_vip_duration</t>
-        </is>
-      </c>
-    </row>
-    <row r="110">
-      <c r="A110" t="inlineStr"/>
-      <c r="B110" t="inlineStr">
-        <is>
-          <t>29 ngày</t>
-        </is>
-      </c>
-      <c r="C110" t="inlineStr"/>
-      <c r="D110" t="inlineStr">
-        <is>
-          <t>enter_data{"duration":"29 ngày"}</t>
-        </is>
-      </c>
-      <c r="E110" t="inlineStr">
-        <is>
-          <t>* enter_data{"duration":"29 ngày"}</t>
-        </is>
-      </c>
-    </row>
-    <row r="111">
-      <c r="A111" t="inlineStr"/>
-      <c r="B111" t="inlineStr"/>
-      <c r="C111" t="inlineStr">
-        <is>
-          <t>slot</t>
-        </is>
-      </c>
-      <c r="D111" t="inlineStr">
-        <is>
-          <t>slot{"duration":"29 ngày"}</t>
-        </is>
-      </c>
-      <c r="E111" t="inlineStr">
-        <is>
-          <t>- slot{"duration":"29 ngày"}</t>
-        </is>
-      </c>
-    </row>
-    <row r="112">
-      <c r="A112" t="inlineStr"/>
-      <c r="B112" t="inlineStr"/>
-      <c r="C112" t="inlineStr">
-        <is>
-          <t>set buy post_package</t>
-        </is>
-      </c>
-      <c r="D112" t="inlineStr">
-        <is>
-          <t>action_set_buy_vip_duration</t>
-        </is>
-      </c>
-      <c r="E112" t="inlineStr">
-        <is>
-          <t>- action_set_buy_vip_duration</t>
-        </is>
-      </c>
-    </row>
-    <row r="113">
-      <c r="A113" t="inlineStr"/>
-      <c r="B113" t="inlineStr"/>
-      <c r="C113" t="inlineStr">
-        <is>
-          <t>Không hợp lệ, nhập lại</t>
-        </is>
-      </c>
-      <c r="D113" t="inlineStr">
-        <is>
-          <t>utter_request_valid_buy_vip_duration</t>
-        </is>
-      </c>
-      <c r="E113" t="inlineStr">
-        <is>
-          <t>- utter_request_valid_buy_vip_duration</t>
-        </is>
-      </c>
-    </row>
-    <row r="114">
-      <c r="A114" t="inlineStr"/>
-      <c r="B114" t="inlineStr">
-        <is>
-          <t>à 30 ngày</t>
-        </is>
-      </c>
-      <c r="C114" t="inlineStr"/>
-      <c r="D114" t="inlineStr">
-        <is>
-          <t>enter_data{"duration":"30 ngày"}</t>
-        </is>
-      </c>
-      <c r="E114" t="inlineStr">
-        <is>
-          <t>* enter_data{"duration":"30 ngày"}</t>
-        </is>
-      </c>
-    </row>
-    <row r="115">
-      <c r="A115" t="inlineStr"/>
-      <c r="B115" t="inlineStr"/>
-      <c r="C115" t="inlineStr">
-        <is>
-          <t>sloot</t>
-        </is>
-      </c>
-      <c r="D115" t="inlineStr">
-        <is>
-          <t>slot{"duration":"30 ngày"}</t>
-        </is>
-      </c>
-      <c r="E115" t="inlineStr">
-        <is>
-          <t>- slot{"duration":"30 ngày"}</t>
-        </is>
-      </c>
-    </row>
-    <row r="116">
-      <c r="A116" t="inlineStr"/>
-      <c r="B116" t="inlineStr"/>
-      <c r="C116" t="inlineStr">
-        <is>
-          <t>set buy post_package</t>
-        </is>
-      </c>
-      <c r="D116" t="inlineStr">
-        <is>
-          <t>action_set_buy_vip_duration</t>
-        </is>
-      </c>
-      <c r="E116" t="inlineStr">
-        <is>
-          <t>- action_set_used_vip_duration</t>
-        </is>
-      </c>
-    </row>
-    <row r="117">
-      <c r="A117" t="inlineStr"/>
-      <c r="B117" t="inlineStr"/>
-      <c r="C117" t="inlineStr">
-        <is>
-          <t>slot</t>
-        </is>
-      </c>
-      <c r="D117" t="inlineStr">
-        <is>
-          <t>slot{"buy_vip_duration":"30 ngày"}</t>
-        </is>
-      </c>
-      <c r="E117" t="inlineStr">
-        <is>
-          <t>- slot{"used_vip_duration":"30 ngày"}</t>
-        </is>
-      </c>
-    </row>
-    <row r="118">
-      <c r="A118" t="inlineStr"/>
-      <c r="B118" t="inlineStr"/>
-      <c r="C118" t="inlineStr">
-        <is>
-          <t>slot</t>
-        </is>
-      </c>
-      <c r="D118" t="inlineStr">
-        <is>
-          <t>slot{"duration":"None"}</t>
-        </is>
-      </c>
-      <c r="E118" t="inlineStr">
-        <is>
-          <t>- slot{"duration":"None"}</t>
-        </is>
-      </c>
-    </row>
-    <row r="119">
-      <c r="A119" t="inlineStr"/>
-      <c r="B119" t="inlineStr"/>
-      <c r="C119" t="inlineStr">
-        <is>
-          <t>Bạn đã dùng được bao nhiêu ngày</t>
-        </is>
-      </c>
-      <c r="D119" t="inlineStr">
-        <is>
-          <t>utter_ask_used_vip_duration</t>
-        </is>
-      </c>
-      <c r="E119" t="inlineStr">
-        <is>
-          <t>- utter_ask_used_vip_duration</t>
-        </is>
-      </c>
-    </row>
-    <row r="120">
-      <c r="A120" t="inlineStr"/>
-      <c r="B120" t="inlineStr">
-        <is>
-          <t>9 ngày rồi</t>
-        </is>
-      </c>
-      <c r="C120" t="inlineStr"/>
-      <c r="D120" t="inlineStr">
-        <is>
-          <t>enter_data{"duration":"9 ngày"}</t>
-        </is>
-      </c>
-      <c r="E120" t="inlineStr"/>
-    </row>
-    <row r="121">
-      <c r="A121" t="inlineStr"/>
-      <c r="B121" t="inlineStr"/>
-      <c r="C121" t="inlineStr">
-        <is>
-          <t>slot</t>
-        </is>
-      </c>
-      <c r="D121" t="inlineStr">
-        <is>
-          <t>slot{"duration":"9 ngày"}</t>
-        </is>
-      </c>
-      <c r="E121" t="inlineStr"/>
-    </row>
-    <row r="122">
-      <c r="A122" t="inlineStr"/>
-      <c r="B122" t="inlineStr"/>
-      <c r="C122" t="inlineStr">
-        <is>
-          <t>action set used vip post</t>
-        </is>
-      </c>
-      <c r="D122" t="inlineStr">
-        <is>
-          <t>action_set_used_vip_duration</t>
-        </is>
-      </c>
-      <c r="E122" t="inlineStr"/>
-    </row>
-    <row r="123">
-      <c r="A123" t="inlineStr"/>
-      <c r="B123" t="inlineStr"/>
-      <c r="C123" t="inlineStr">
-        <is>
-          <t>slot</t>
-        </is>
-      </c>
-      <c r="D123" t="inlineStr">
-        <is>
-          <t>slot{"used_vip_duration":"9 ngày"}</t>
-        </is>
-      </c>
-      <c r="E123" t="inlineStr"/>
-    </row>
-    <row r="124">
-      <c r="A124" t="inlineStr"/>
-      <c r="B124" t="inlineStr"/>
-      <c r="C124" t="inlineStr">
-        <is>
-          <t>slot</t>
-        </is>
-      </c>
-      <c r="D124" t="inlineStr">
-        <is>
-          <t>slot{"duration":"None"}</t>
-        </is>
-      </c>
-      <c r="E124" t="inlineStr"/>
-    </row>
-    <row r="125">
-      <c r="A125" t="inlineStr"/>
-      <c r="B125" t="inlineStr"/>
-      <c r="C125" t="inlineStr">
-        <is>
-          <t>action utter</t>
-        </is>
-      </c>
-      <c r="D125" t="inlineStr">
-        <is>
-          <t>action_calculate_down_post</t>
-        </is>
-      </c>
-      <c r="E125" t="inlineStr"/>
-    </row>
-    <row r="126">
-      <c r="A126" t="inlineStr"/>
-      <c r="B126" t="inlineStr">
-        <is>
-          <t>cách tính chi tiết như nào thế</t>
-        </is>
-      </c>
-      <c r="C126" t="inlineStr"/>
-      <c r="D126" t="inlineStr">
-        <is>
-          <t>request_more</t>
-        </is>
-      </c>
-      <c r="E126" t="inlineStr"/>
-    </row>
-    <row r="127">
-      <c r="A127" t="inlineStr"/>
-      <c r="B127" t="inlineStr"/>
-      <c r="C127" t="inlineStr">
-        <is>
-          <t>Xin lỗi, bot chỉ hỗ trợ bạn được như vậy thôi ạ!</t>
-        </is>
-      </c>
-      <c r="D127" t="inlineStr">
-        <is>
-          <t>utter_out_of_bot_ability</t>
-        </is>
-      </c>
-      <c r="E127" t="inlineStr"/>
-    </row>
-    <row r="128">
-      <c r="A128" t="inlineStr"/>
-      <c r="B128" t="inlineStr"/>
-      <c r="C128" t="inlineStr">
-        <is>
-          <t>Bạn liên hệ để được hỗ trợ nâng cao:
-• Gọi đến tổng đài theo số hotline 08.69.09.29.29
-• Gửi mail yêu cầu hỗ trợ tới địa chỉ “contact@meeyland.com”
-• Chat với "Chăm sóc khách hàng"</t>
-        </is>
-      </c>
-      <c r="D128" t="inlineStr">
-        <is>
-          <t>utter_how_contact_customer_service</t>
-        </is>
-      </c>
-      <c r="E128" t="inlineStr"/>
+          <t>- utter_anything_else</t>
+        </is>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>